<commit_message>
Re-ran 57 system again, accuracy is higher
</commit_message>
<xml_diff>
--- a/RESULTS_IEEE57_ClassifiersTest.xlsx
+++ b/RESULTS_IEEE57_ClassifiersTest.xlsx
@@ -449,19 +449,19 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.6105</v>
+        <v>0.4975</v>
       </c>
       <c r="D2">
-        <v>0.6895177361498604</v>
+        <v>0.6639919759277833</v>
       </c>
       <c r="E2">
-        <v>0.5732273028495692</v>
+        <v>0.4987443495730788</v>
       </c>
       <c r="F2">
-        <v>0.865</v>
+        <v>0.993</v>
       </c>
       <c r="G2">
-        <v>0.644</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -472,19 +472,19 @@
         <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0.4925</v>
+        <v>0.483</v>
       </c>
       <c r="D3">
-        <v>0.6590527376553578</v>
+        <v>0.6492537313432836</v>
       </c>
       <c r="E3">
-        <v>0.496206373292868</v>
+        <v>0.4912731006160164</v>
       </c>
       <c r="F3">
-        <v>0.981</v>
+        <v>0.957</v>
       </c>
       <c r="G3">
-        <v>0.996</v>
+        <v>0.991</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -495,19 +495,19 @@
         <v>0.3</v>
       </c>
       <c r="C4">
-        <v>0.486</v>
+        <v>0.4975</v>
       </c>
       <c r="D4">
-        <v>0.6538720538720538</v>
+        <v>0.6639919759277833</v>
       </c>
       <c r="E4">
-        <v>0.4928934010152284</v>
+        <v>0.4987443495730788</v>
       </c>
       <c r="F4">
-        <v>0.971</v>
+        <v>0.993</v>
       </c>
       <c r="G4">
-        <v>0.999</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -518,19 +518,19 @@
         <v>0.4</v>
       </c>
       <c r="C5">
-        <v>0.4915</v>
+        <v>0.4985</v>
       </c>
       <c r="D5">
-        <v>0.6588393156658838</v>
+        <v>0.6639865996649916</v>
       </c>
       <c r="E5">
-        <v>0.4957092377587077</v>
+        <v>0.4992443324937028</v>
       </c>
       <c r="F5">
-        <v>0.982</v>
+        <v>0.991</v>
       </c>
       <c r="G5">
-        <v>0.999</v>
+        <v>0.994</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -541,19 +541,19 @@
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>0.5034999999999999</v>
+        <v>0.634</v>
       </c>
       <c r="D6">
-        <v>0.666218487394958</v>
+        <v>0.7306843267108168</v>
       </c>
       <c r="E6">
-        <v>0.5017721518987341</v>
+        <v>0.5779976717112922</v>
       </c>
       <c r="F6">
-        <v>0.991</v>
+        <v>0.993</v>
       </c>
       <c r="G6">
-        <v>0.984</v>
+        <v>0.725</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -564,19 +564,19 @@
         <v>0.6</v>
       </c>
       <c r="C7">
-        <v>0.4975</v>
+        <v>0.4995</v>
       </c>
       <c r="D7">
-        <v>0.664440734557596</v>
+        <v>0.6639812017455521</v>
       </c>
       <c r="E7">
-        <v>0.4987468671679198</v>
+        <v>0.4997473471450227</v>
       </c>
       <c r="F7">
-        <v>0.995</v>
+        <v>0.989</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -587,19 +587,19 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="C8">
-        <v>0.494</v>
+        <v>0.4995</v>
       </c>
       <c r="D8">
-        <v>0.6613119143239624</v>
+        <v>0.6657762938230384</v>
       </c>
       <c r="E8">
-        <v>0.4969818913480885</v>
+        <v>0.4997493734335839</v>
       </c>
       <c r="F8">
-        <v>0.988</v>
+        <v>0.997</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -610,19 +610,19 @@
         <v>0.8</v>
       </c>
       <c r="C9">
-        <v>0.5135</v>
+        <v>0.498</v>
       </c>
       <c r="D9">
-        <v>0.6725008414675194</v>
+        <v>0.6639892904953146</v>
       </c>
       <c r="E9">
-        <v>0.5068493150684932</v>
+        <v>0.4989939637826962</v>
       </c>
       <c r="F9">
-        <v>0.999</v>
+        <v>0.992</v>
       </c>
       <c r="G9">
-        <v>0.972</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -633,19 +633,19 @@
         <v>0.9</v>
       </c>
       <c r="C10">
-        <v>0.9429999999999999</v>
+        <v>0.5065</v>
       </c>
       <c r="D10">
-        <v>0.9459203036053131</v>
+        <v>0.6682352941176469</v>
       </c>
       <c r="E10">
-        <v>0.8998194945848376</v>
+        <v>0.5032911392405063</v>
       </c>
       <c r="F10">
-        <v>0.997</v>
+        <v>0.994</v>
       </c>
       <c r="G10">
-        <v>0.111</v>
+        <v>0.981</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -656,19 +656,19 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.495</v>
+        <v>0.9305</v>
       </c>
       <c r="D11">
-        <v>0.6622073578595318</v>
+        <v>0.9253891572732152</v>
       </c>
       <c r="E11">
-        <v>0.4974874371859296</v>
+        <v>0.9988412514484357</v>
       </c>
       <c r="F11">
-        <v>0.99</v>
+        <v>0.862</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0.001</v>
       </c>
     </row>
   </sheetData>
@@ -735,19 +735,19 @@
         <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0.505</v>
+        <v>0.5</v>
       </c>
       <c r="D3">
-        <v>0.6688963210702341</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E3">
-        <v>0.5025125628140703</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -758,19 +758,19 @@
         <v>0.3</v>
       </c>
       <c r="C4">
-        <v>0.9805</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
-        <v>0.9808729769494851</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E4">
-        <v>0.9624639076034649</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0.039</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -781,19 +781,19 @@
         <v>0.4</v>
       </c>
       <c r="C5">
-        <v>0.8090000000000001</v>
+        <v>0.9845</v>
       </c>
       <c r="D5">
-        <v>0.8396305625524769</v>
+        <v>0.9847365829640571</v>
       </c>
       <c r="E5">
-        <v>0.723589001447178</v>
+        <v>0.9699321047526673</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>0.382</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -804,19 +804,19 @@
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>0.967</v>
+        <v>0.5</v>
       </c>
       <c r="D6">
-        <v>0.968054211035818</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E6">
-        <v>0.9380863039399625</v>
+        <v>0.5</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.066</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -827,19 +827,19 @@
         <v>0.6</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>0.9885</v>
       </c>
       <c r="D7">
-        <v>0.6666666666666666</v>
+        <v>0.9886307464162135</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0.9775171065493646</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -850,19 +850,19 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="C8">
-        <v>0.9845</v>
+        <v>0.5</v>
       </c>
       <c r="D8">
-        <v>0.9847365829640571</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E8">
-        <v>0.9699321047526673</v>
+        <v>0.5</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
-        <v>0.031</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -873,19 +873,19 @@
         <v>0.8</v>
       </c>
       <c r="C9">
-        <v>0.99</v>
+        <v>0.958</v>
       </c>
       <c r="D9">
-        <v>0.99009900990099</v>
+        <v>0.9596928982725529</v>
       </c>
       <c r="E9">
-        <v>0.9803921568627451</v>
+        <v>0.922509225092251</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
-        <v>0.02</v>
+        <v>0.08400000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -896,19 +896,19 @@
         <v>0.9</v>
       </c>
       <c r="C10">
-        <v>0.9845</v>
+        <v>0.9035</v>
       </c>
       <c r="D10">
-        <v>0.9847365829640571</v>
+        <v>0.9119927040583675</v>
       </c>
       <c r="E10">
-        <v>0.9699321047526673</v>
+        <v>0.8382229673093042</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0.031</v>
+        <v>0.193</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -919,19 +919,19 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0.524</v>
       </c>
       <c r="D11">
-        <v>0.6666666666666666</v>
+        <v>0.6775067750677507</v>
       </c>
       <c r="E11">
-        <v>0.5</v>
+        <v>0.5122950819672131</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0.952</v>
       </c>
     </row>
   </sheetData>
@@ -975,19 +975,19 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.6895</v>
+        <v>0.782</v>
       </c>
       <c r="D2">
-        <v>0.5509761388286334</v>
+        <v>0.7212276214833758</v>
       </c>
       <c r="E2">
-        <v>0.9947780678851175</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0.381</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="G2">
-        <v>0.002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -998,19 +998,19 @@
         <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0.72</v>
+        <v>0.8725000000000001</v>
       </c>
       <c r="D3">
-        <v>0.6116504854368932</v>
+        <v>0.8843537414965986</v>
       </c>
       <c r="E3">
-        <v>0.997737556561086</v>
+        <v>0.8091286307053942</v>
       </c>
       <c r="F3">
-        <v>0.441</v>
+        <v>0.975</v>
       </c>
       <c r="G3">
-        <v>0.001</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1021,16 +1021,16 @@
         <v>0.3</v>
       </c>
       <c r="C4">
-        <v>0.8345</v>
+        <v>0.9495</v>
       </c>
       <c r="D4">
-        <v>0.8016776512881966</v>
+        <v>0.94681411269089</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0.669</v>
+        <v>0.899</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1044,16 +1044,16 @@
         <v>0.4</v>
       </c>
       <c r="C5">
-        <v>0.8804999999999999</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="D5">
-        <v>0.8642816581487791</v>
+        <v>0.9327641408751334</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.761</v>
+        <v>0.874</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1067,16 +1067,16 @@
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>0.9375</v>
+        <v>0.9825</v>
       </c>
       <c r="D6">
-        <v>0.9333333333333333</v>
+        <v>0.9821882951653944</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>0.875</v>
+        <v>0.965</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1090,19 +1090,19 @@
         <v>0.6</v>
       </c>
       <c r="C7">
-        <v>0.984</v>
+        <v>0.982</v>
       </c>
       <c r="D7">
-        <v>0.984</v>
+        <v>0.9816700610997963</v>
       </c>
       <c r="E7">
-        <v>0.984</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0.984</v>
+        <v>0.964</v>
       </c>
       <c r="G7">
-        <v>0.016</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1113,19 +1113,19 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="C8">
-        <v>0.964</v>
+        <v>0.954</v>
       </c>
       <c r="D8">
-        <v>0.9627329192546584</v>
+        <v>0.9517819706498952</v>
       </c>
       <c r="E8">
-        <v>0.9978540772532188</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0.93</v>
+        <v>0.908</v>
       </c>
       <c r="G8">
-        <v>0.002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1136,16 +1136,16 @@
         <v>0.8</v>
       </c>
       <c r="C9">
-        <v>0.98</v>
+        <v>0.9325</v>
       </c>
       <c r="D9">
-        <v>0.9795918367346939</v>
+        <v>0.9276139410187667</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0.96</v>
+        <v>0.865</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1159,16 +1159,16 @@
         <v>0.9</v>
       </c>
       <c r="C10">
-        <v>0.9855</v>
+        <v>0.9835</v>
       </c>
       <c r="D10">
-        <v>0.9852866565195332</v>
+        <v>0.9832231825114387</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0.971</v>
+        <v>0.967</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1182,16 +1182,16 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.9965000000000001</v>
+        <v>0.984</v>
       </c>
       <c r="D11">
-        <v>0.9964877069744105</v>
+        <v>0.983739837398374</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>0.993</v>
+        <v>0.968</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1238,19 +1238,19 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.499</v>
+        <v>0.5315</v>
       </c>
       <c r="D2">
-        <v>0.6657771847898599</v>
+        <v>0.1185324553151458</v>
       </c>
       <c r="E2">
-        <v>0.4994994994994995</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0.998</v>
+        <v>0.063</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1261,19 +1261,19 @@
         <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.5004999999999999</v>
       </c>
       <c r="D3">
-        <v>0.6666666666666666</v>
+        <v>0.6668889629876625</v>
       </c>
       <c r="E3">
-        <v>0.5</v>
+        <v>0.5002501250625313</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1284,19 +1284,19 @@
         <v>0.3</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0.997</v>
       </c>
       <c r="D4">
-        <v>0.6666666666666666</v>
+        <v>0.997002997002997</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>0.9960079840319361</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1307,19 +1307,19 @@
         <v>0.4</v>
       </c>
       <c r="C5">
-        <v>0.9825</v>
+        <v>0.9565</v>
       </c>
       <c r="D5">
-        <v>0.9827840629611411</v>
+        <v>0.9545216936748563</v>
       </c>
       <c r="E5">
-        <v>0.9670861568247822</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0.999</v>
+        <v>0.913</v>
       </c>
       <c r="G5">
-        <v>0.034</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1330,19 +1330,19 @@
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>0.998</v>
+        <v>0.5004999999999999</v>
       </c>
       <c r="D6">
-        <v>0.998001998001998</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="E6">
-        <v>0.9970059880239521</v>
+        <v>0.5002503755633451</v>
       </c>
       <c r="F6">
         <v>0.999</v>
       </c>
       <c r="G6">
-        <v>0.003</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1353,19 +1353,19 @@
         <v>0.6</v>
       </c>
       <c r="C7">
-        <v>0.4995</v>
+        <v>0.9985000000000001</v>
       </c>
       <c r="D7">
-        <v>0.6662220740246749</v>
+        <v>0.99849774661993</v>
       </c>
       <c r="E7">
-        <v>0.4997498749374688</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0.999</v>
+        <v>0.997</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1376,16 +1376,16 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="C8">
-        <v>0.999</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0.998998998998999</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>0.998</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1399,16 +1399,16 @@
         <v>0.8</v>
       </c>
       <c r="C9">
-        <v>0.999</v>
+        <v>0.9955000000000001</v>
       </c>
       <c r="D9">
-        <v>0.998998998998999</v>
+        <v>0.9954796584630838</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0.998</v>
+        <v>0.991</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1422,16 +1422,16 @@
         <v>0.9</v>
       </c>
       <c r="C10">
-        <v>0.9995000000000001</v>
+        <v>0.9935</v>
       </c>
       <c r="D10">
-        <v>0.9994997498749374</v>
+        <v>0.9934574735782586</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0.999</v>
+        <v>0.987</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1445,16 +1445,16 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.995</v>
+        <v>0.996</v>
       </c>
       <c r="D11">
-        <v>0.9949748743718593</v>
+        <v>0.9959839357429718</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>0.99</v>
+        <v>0.992</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1501,19 +1501,19 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.654</v>
+        <v>0.548</v>
       </c>
       <c r="D2">
-        <v>0.4733637747336378</v>
+        <v>0.1751824817518248</v>
       </c>
       <c r="E2">
-        <v>0.9904458598726115</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0.311</v>
+        <v>0.096</v>
       </c>
       <c r="G2">
-        <v>0.003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1524,19 +1524,19 @@
         <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0.905</v>
+        <v>0.983</v>
       </c>
       <c r="D3">
-        <v>0.8957189901207464</v>
+        <v>0.983184965380811</v>
       </c>
       <c r="E3">
-        <v>0.9927007299270073</v>
+        <v>0.9726027397260274</v>
       </c>
       <c r="F3">
-        <v>0.8159999999999999</v>
+        <v>0.994</v>
       </c>
       <c r="G3">
-        <v>0.006</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1547,19 +1547,19 @@
         <v>0.3</v>
       </c>
       <c r="C4">
-        <v>0.977</v>
+        <v>0.972</v>
       </c>
       <c r="D4">
-        <v>0.976482617586912</v>
+        <v>0.971252566735113</v>
       </c>
       <c r="E4">
-        <v>0.9989539748953975</v>
+        <v>0.9978902953586498</v>
       </c>
       <c r="F4">
-        <v>0.955</v>
+        <v>0.946</v>
       </c>
       <c r="G4">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1570,16 +1570,16 @@
         <v>0.4</v>
       </c>
       <c r="C5">
-        <v>0.969</v>
+        <v>0.948</v>
       </c>
       <c r="D5">
-        <v>0.9680082559339525</v>
+        <v>0.9451476793248946</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.9379999999999999</v>
+        <v>0.896</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1593,19 +1593,19 @@
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>0.997</v>
+        <v>0.995</v>
       </c>
       <c r="D6">
-        <v>0.997</v>
+        <v>0.9950199203187251</v>
       </c>
       <c r="E6">
-        <v>0.997</v>
+        <v>0.9910714285714286</v>
       </c>
       <c r="F6">
-        <v>0.997</v>
+        <v>0.999</v>
       </c>
       <c r="G6">
-        <v>0.003</v>
+        <v>0.008999999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1616,19 +1616,19 @@
         <v>0.6</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>0.9965000000000001</v>
       </c>
       <c r="D7">
-        <v>0.6664442961974649</v>
+        <v>0.9964877069744105</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0.999</v>
+        <v>0.993</v>
       </c>
       <c r="G7">
-        <v>0.999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1639,16 +1639,16 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="C8">
-        <v>0.99</v>
+        <v>0.9995000000000001</v>
       </c>
       <c r="D8">
-        <v>0.9898989898989899</v>
+        <v>0.9994997498749374</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>0.98</v>
+        <v>0.999</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1662,16 +1662,16 @@
         <v>0.8</v>
       </c>
       <c r="C9">
-        <v>0.9975000000000001</v>
+        <v>0.993</v>
       </c>
       <c r="D9">
-        <v>0.9974937343358395</v>
+        <v>0.9929506545820745</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0.995</v>
+        <v>0.986</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1685,16 +1685,16 @@
         <v>0.9</v>
       </c>
       <c r="C10">
-        <v>0.9995000000000001</v>
+        <v>0.993</v>
       </c>
       <c r="D10">
-        <v>0.9994997498749374</v>
+        <v>0.9929506545820745</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0.999</v>
+        <v>0.986</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1708,16 +1708,16 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.995</v>
+        <v>0.993</v>
       </c>
       <c r="D11">
-        <v>0.9949748743718593</v>
+        <v>0.9929506545820745</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>0.99</v>
+        <v>0.986</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1752,7 +1752,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>78.6681547164917</v>
+        <v>66.77434110641479</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1763,7 +1763,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>2.484050989151001</v>
+        <v>3.152542352676392</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1774,7 +1774,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>0.6722018718719482</v>
+        <v>0.8976325988769531</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1785,7 +1785,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>156.866730928421</v>
+        <v>143.1019971370697</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1796,7 +1796,7 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>1168.711619377136</v>
+        <v>2537.503065347672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>